<commit_message>
updates to graph script to compute the current day. updates to pid trend stats
</commit_message>
<xml_diff>
--- a/charts/PID_counts_varying_status_age.xlsx
+++ b/charts/PID_counts_varying_status_age.xlsx
@@ -118,6 +118,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>25-Oct</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> to 7-Nov</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -177,10 +197,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>25</c:v>
@@ -192,10 +212,10 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -252,10 +272,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18</c:v>
@@ -267,10 +287,10 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>65</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,10 +347,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>21</c:v>
@@ -342,10 +362,10 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>68</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,11 +382,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="79345152"/>
-        <c:axId val="76378112"/>
+        <c:axId val="54760960"/>
+        <c:axId val="54762496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79345152"/>
+        <c:axId val="54760960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,7 +395,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76378112"/>
+        <c:crossAx val="54762496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -383,7 +403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76378112"/>
+        <c:axId val="54762496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +413,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79345152"/>
+        <c:crossAx val="54760960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -427,8 +447,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -739,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,13 +789,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -783,13 +803,13 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -839,13 +859,13 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D7">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E7">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -853,13 +873,13 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D8">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E8">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>